<commit_message>
successfully managed to read from excel
</commit_message>
<xml_diff>
--- a/Excels/basic.xlsx
+++ b/Excels/basic.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Dallash\Documents\GitHub\Advanced-Computer-Programming-Final-Projest\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Dallash\Documents\GitHub\Advanced-Computer-Programming-Final-Project\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D5BBD9-8C7C-4A2E-B015-03DB2513E02F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BC65B2-9802-4FE7-8304-02A18D403F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="19200" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2220" yWindow="1884" windowWidth="19200" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>A1</t>
-  </si>
-  <si>
     <t>B1</t>
   </si>
   <si>
@@ -37,6 +34,9 @@
   </si>
   <si>
     <t>B2</t>
+  </si>
+  <si>
+    <t>A1296299</t>
   </si>
 </sst>
 </file>
@@ -356,26 +356,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last commit before adding the mend
</commit_message>
<xml_diff>
--- a/Excels/basic.xlsx
+++ b/Excels/basic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Dallash\Documents\GitHub\Advanced-Computer-Programming-Final-Project\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA26C34-54D8-4218-A585-57BA2D949CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F2597F-46E8-4412-AA7F-18B9DE46D2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="19200" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>/object1/field1</t>
   </si>
@@ -79,6 +79,33 @@
   </si>
   <si>
     <t>object5</t>
+  </si>
+  <si>
+    <t>/field12</t>
+  </si>
+  <si>
+    <t>/object3</t>
+  </si>
+  <si>
+    <t>object3</t>
+  </si>
+  <si>
+    <t>/object3/field12</t>
+  </si>
+  <si>
+    <t>/object3/object4</t>
+  </si>
+  <si>
+    <t>object4</t>
+  </si>
+  <si>
+    <t>/object3/object4/field13</t>
+  </si>
+  <si>
+    <t>/object3/object4/field14</t>
+  </si>
+  <si>
+    <t>/object5/field15</t>
   </si>
 </sst>
 </file>
@@ -452,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,11 +606,67 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B20" s="3" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mandatory and allowed values are added
</commit_message>
<xml_diff>
--- a/Excels/basic.xlsx
+++ b/Excels/basic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Dallash\Documents\GitHub\Advanced-Computer-Programming-Final-Project\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D060F8D-4F98-47D2-9975-E5736BA9FC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB77C09-4DD5-40E0-8D7E-C8DD669AFA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="34">
   <si>
     <t>/object1/field1</t>
   </si>
@@ -112,6 +112,21 @@
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>Y,N</t>
+  </si>
+  <si>
+    <t>0,1</t>
   </si>
 </sst>
 </file>
@@ -121,7 +136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +167,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -162,12 +193,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -175,63 +206,32 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -514,278 +514,379 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.21875" customWidth="1"/>
-    <col min="2" max="2" width="42.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="12" t="s">
+      <c r="C5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="11" t="s">
+      <c r="C7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="C8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="C9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="C10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="11" t="s">
+      <c r="C11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="11" t="s">
+      <c r="C12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="11" t="s">
+      <c r="C13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+      <c r="C14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
+      <c r="C16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="C18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="C19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
+      <c r="C21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="8"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="8"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
       <c r="C27" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working but with no array
</commit_message>
<xml_diff>
--- a/Excels/basic.xlsx
+++ b/Excels/basic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Dallash\Documents\GitHub\Advanced-Computer-Programming-Final-Project\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB77C09-4DD5-40E0-8D7E-C8DD669AFA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DCC681-ED99-4F06-AEBD-496FBAEBAA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="11580" windowWidth="19200" windowHeight="9792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="44">
   <si>
     <t>/object1/field1</t>
   </si>
@@ -127,6 +127,36 @@
   </si>
   <si>
     <t>0,1</t>
+  </si>
+  <si>
+    <t>REST Operation Mapping (API_NAME)</t>
+  </si>
+  <si>
+    <t>HTTP Operation</t>
+  </si>
+  <si>
+    <t>REST URL</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>/somePath/somePath2</t>
+  </si>
+  <si>
+    <t>I/o</t>
+  </si>
+  <si>
+    <t>Field Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Allowed Values</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
   </si>
 </sst>
 </file>
@@ -145,12 +175,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Franklin Gothic Book"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -160,12 +184,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -182,6 +200,20 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -209,28 +241,42 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -516,381 +562,388 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="36.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="47.88671875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="D7" s="11"/>
+      <c r="E7" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="C8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7" t="s">
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="6" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="C13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E13" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="6" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E14" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="6" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
+      <c r="C15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="6" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7" t="s">
+      <c r="C16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="6" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7" t="s">
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="6" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="C18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="E19" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="D21" s="11"/>
+      <c r="E21" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="D23" s="11"/>
+      <c r="E23" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="C24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="C25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7" t="s">
+      <c r="D26" s="11"/>
+      <c r="E26" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="2"/>
+      <c r="C27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
working for the first
</commit_message>
<xml_diff>
--- a/Excels/basic.xlsx
+++ b/Excels/basic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Dallash\Documents\GitHub\Advanced-Computer-Programming-Final-Project\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DCC681-ED99-4F06-AEBD-496FBAEBAA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260E4D75-9540-4148-9530-BB0ED0DF87DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="11580" windowWidth="19200" windowHeight="9792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -560,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -942,6 +942,180 @@
         <v>29</v>
       </c>
     </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="12"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="12"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="12"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="12"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="12"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="12"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="12"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="12"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="12"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="12"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="12"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="12"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="12"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="12"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="4"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="12"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="4"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="12"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="4"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="12"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="4"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="12"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="4"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="12"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="4"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="12"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="4"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="12"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
make the iterator move automatically
</commit_message>
<xml_diff>
--- a/Excels/basic.xlsx
+++ b/Excels/basic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Dallash\Documents\GitHub\Advanced-Computer-Programming-Final-Project\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260E4D75-9540-4148-9530-BB0ED0DF87DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AA2DF4-E475-4E75-AF93-8257B0EA11EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -230,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -238,12 +238,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -255,28 +270,44 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -560,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:F56"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,550 +602,630 @@
     <col min="1" max="1" width="36.109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="47.88671875" style="3" customWidth="1"/>
     <col min="3" max="3" width="15.21875" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="3"/>
+    <col min="4" max="4" width="19.21875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="C8" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="C9" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="C10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12" t="s">
+      <c r="C11" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="D12" s="16"/>
+      <c r="E12" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="11" t="s">
+      <c r="C13" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="11" t="s">
+      <c r="C14" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12" t="s">
+      <c r="C15" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12" t="s">
+      <c r="C16" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12" t="s">
+      <c r="C17" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="C18" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="11" t="s">
+      <c r="C19" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="E19" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="C20" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="D21" s="16"/>
+      <c r="E21" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="C22" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="D23" s="16"/>
+      <c r="E23" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="C24" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="C25" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="12" t="s">
+      <c r="D26" s="16"/>
+      <c r="E26" s="17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="12"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="12"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="12"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="12"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="12"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="12"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="12"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C27" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="12"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="14"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="14"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="14"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="14"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="14"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="14"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="14"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="12"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D42" s="5"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="12"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D43" s="5"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="12"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D44" s="5"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="12"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D45" s="5"/>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="12"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D46" s="5"/>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="12"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D47" s="5"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="12"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="6"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="2"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="12"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="6"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="2"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="12"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="6"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="2"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="12"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="6"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="2"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="12"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="6"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="B53" s="2"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="12"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="6"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="2"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="12"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="6"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="2"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="12"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>